<commit_message>
Testdaten hinzugefügt + Getter und Setter durch Lombok ersetzt + versucht Controller durch automatische REST generation zu ersetzen
</commit_message>
<xml_diff>
--- a/externe dateien/TodoListe Projekt.xlsx
+++ b/externe dateien/TodoListe Projekt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bbwch-my.sharepoint.com/personal/kevin_luethi_lernende_bbw_ch/Documents/1Lehrjahr/AXA/persistence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\axakurse\persistenceprojekt\externe dateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{05B85CE6-7FE2-47CF-8CFE-A8FB73E37DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED93DF9C-7C0D-48E5-AAC1-B802AC119D97}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4211B9-B9BB-46A0-8923-556CCE195637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{26523A63-A4C8-4DF5-880F-14DB076CA917}"/>
   </bookViews>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A35FA0-9F22-43B6-A1C4-5EE8F4527E57}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -760,7 +760,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -768,7 +768,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -776,7 +776,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -784,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -792,7 +792,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="24" x14ac:dyDescent="0.4">
@@ -990,9 +990,6 @@
       <c r="A64" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B64" s="4" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="65" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
@@ -1007,7 +1004,7 @@
         <v>48</v>
       </c>
       <c r="B66" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -1015,7 +1012,7 @@
         <v>50</v>
       </c>
       <c r="B67" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -1023,7 +1020,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -1037,6 +1034,9 @@
     <row r="70" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="B70" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="24" x14ac:dyDescent="0.4">

</xml_diff>